<commit_message>
Updated data files and some simple analyses
</commit_message>
<xml_diff>
--- a/data/submittedround6/grephon table Alana and Cat final round.xlsx
+++ b/data/submittedround6/grephon table Alana and Cat final round.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.chamberlain/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2A5E04-F87D-DD44-B4AB-B79207DE7204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2738EE2-5AFF-8143-8865-AA29582E8D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="760" windowWidth="30880" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="217">
   <si>
     <t>paper_id</t>
   </si>
@@ -275,9 +275,6 @@
     <t>negative relationship</t>
   </si>
   <si>
-    <t>notsure</t>
-  </si>
-  <si>
     <t xml:space="preserve"> biomass</t>
   </si>
   <si>
@@ -702,6 +699,12 @@
   </si>
   <si>
     <t>They're more interested in phenological ranks and how earlier leafout species take advantage of early spring resources and grow more and then later leafout species have end of season resources and grow more but they did find a weak relationship between longer gsl and growth for two out of the three species</t>
+  </si>
+  <si>
+    <t>gs_metric_other</t>
+  </si>
+  <si>
+    <t>no data for this</t>
   </si>
 </sst>
 </file>
@@ -1528,19 +1531,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR15"/>
+  <dimension ref="A1:AS15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP18" sqref="AP18"/>
+      <selection activeCell="R13" sqref="R13:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="11" max="12" width="11.83203125" customWidth="1"/>
-    <col min="33" max="33" width="12.1640625" customWidth="1"/>
+    <col min="34" max="34" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1596,85 +1599,88 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
+        <v>215</v>
+      </c>
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
         <v>62</v>
@@ -1730,76 +1736,79 @@
         <v>66</v>
       </c>
       <c r="S2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="U2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" t="s">
         <v>67</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>70</v>
       </c>
-      <c r="W2" t="s">
-        <v>62</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>62</v>
+      <c r="X2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Z2" t="s">
         <v>62</v>
       </c>
       <c r="AA2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="AB2" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="AC2" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="AD2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AE2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AF2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AG2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="AH2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="AI2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AJ2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AK2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AL2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM2" t="s">
         <v>49</v>
       </c>
-      <c r="AM2" t="s">
-        <v>68</v>
-      </c>
       <c r="AN2" t="s">
         <v>68</v>
       </c>
       <c r="AO2" t="s">
-        <v>79</v>
+        <v>68</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1831,7 +1840,7 @@
         <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L3" t="s">
         <v>60</v>
@@ -1854,77 +1863,80 @@
       <c r="R3" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="T3" t="s">
-        <v>62</v>
-      </c>
       <c r="U3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" t="s">
         <v>69</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>71</v>
       </c>
-      <c r="W3" t="s">
-        <v>62</v>
-      </c>
       <c r="X3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="Y3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="Z3" t="s">
         <v>62</v>
       </c>
       <c r="AA3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AB3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="AC3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AD3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AE3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AF3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AG3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="AH3" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="AI3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AJ3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AK3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AL3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM3" t="s">
         <v>49</v>
       </c>
-      <c r="AM3" t="s">
-        <v>68</v>
-      </c>
       <c r="AN3" t="s">
         <v>68</v>
       </c>
-      <c r="AQ3" t="s">
-        <v>75</v>
+      <c r="AO3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -2010,51 +2022,54 @@
         <v>62</v>
       </c>
       <c r="AC4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AD4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AE4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AF4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AG4" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="AH4" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="AI4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AJ4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AK4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AL4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM4" t="s">
         <v>49</v>
       </c>
-      <c r="AM4" t="s">
-        <v>68</v>
-      </c>
       <c r="AN4" t="s">
         <v>68</v>
       </c>
+      <c r="AO4" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
@@ -2063,34 +2078,34 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
         <v>82</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>83</v>
-      </c>
-      <c r="H5" t="s">
-        <v>84</v>
       </c>
       <c r="I5" t="s">
         <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" t="s">
         <v>85</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>86</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" t="s">
         <v>87</v>
-      </c>
-      <c r="N5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" t="s">
-        <v>88</v>
       </c>
       <c r="P5" t="s">
         <v>62</v>
@@ -2102,203 +2117,209 @@
         <v>66</v>
       </c>
       <c r="S5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="T5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="U5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="V5" t="s">
+        <v>68</v>
+      </c>
+      <c r="W5" t="s">
+        <v>89</v>
+      </c>
+      <c r="X5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA5" t="s">
         <v>90</v>
       </c>
-      <c r="W5" t="s">
-        <v>62</v>
-      </c>
-      <c r="X5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH5" t="s">
         <v>91</v>
       </c>
-      <c r="AA5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG5" t="s">
+      <c r="AI5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>92</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
         <v>95</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" t="s">
         <v>96</v>
       </c>
-      <c r="H6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>97</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>98</v>
       </c>
-      <c r="K6" t="s">
-        <v>99</v>
-      </c>
       <c r="L6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
         <v>101</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" t="s">
         <v>102</v>
       </c>
-      <c r="N6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T6" t="s">
+        <v>68</v>
+      </c>
+      <c r="U6" t="s">
+        <v>62</v>
+      </c>
+      <c r="V6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W6" t="s">
+        <v>62</v>
+      </c>
+      <c r="X6" t="s">
         <v>103</v>
       </c>
-      <c r="P6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>64</v>
-      </c>
-      <c r="R6" t="s">
-        <v>62</v>
-      </c>
-      <c r="S6" t="s">
-        <v>68</v>
-      </c>
-      <c r="T6" t="s">
-        <v>62</v>
-      </c>
-      <c r="U6" t="s">
-        <v>62</v>
-      </c>
-      <c r="V6" t="s">
-        <v>62</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA6" t="s">
         <v>104</v>
       </c>
-      <c r="X6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>68</v>
-      </c>
       <c r="AB6" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="AC6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AD6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AE6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AF6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AG6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR6" t="s">
         <v>107</v>
       </c>
-      <c r="AH6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ6" t="s">
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>109</v>
-      </c>
-      <c r="B7" t="s">
-        <v>110</v>
       </c>
       <c r="C7" t="s">
         <v>58</v>
@@ -2310,25 +2331,25 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" t="s">
         <v>112</v>
-      </c>
-      <c r="G7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H7" t="s">
-        <v>113</v>
       </c>
       <c r="I7" t="s">
         <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K7" t="s">
         <v>59</v>
       </c>
       <c r="L7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M7" t="s">
         <v>61</v>
@@ -2349,84 +2370,87 @@
         <v>66</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="U7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="V7" t="s">
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="W7" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="X7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Y7" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="Z7" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="AA7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AB7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AC7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AD7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AE7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="AF7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AG7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM7" t="s">
         <v>138</v>
       </c>
-      <c r="AH7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL7" t="s">
+      <c r="AN7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP7" t="s">
         <v>139</v>
       </c>
-      <c r="AM7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>131</v>
+      <c r="AR7" t="s">
+        <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
         <v>109</v>
-      </c>
-      <c r="B8" t="s">
-        <v>110</v>
       </c>
       <c r="C8" t="s">
         <v>58</v>
@@ -2438,25 +2462,25 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" t="s">
         <v>112</v>
-      </c>
-      <c r="G8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" t="s">
-        <v>113</v>
       </c>
       <c r="I8" t="s">
         <v>55</v>
       </c>
       <c r="J8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" t="s">
         <v>114</v>
-      </c>
-      <c r="K8" t="s">
-        <v>118</v>
-      </c>
-      <c r="L8" t="s">
-        <v>115</v>
       </c>
       <c r="M8" t="s">
         <v>61</v>
@@ -2477,84 +2501,87 @@
         <v>66</v>
       </c>
       <c r="S8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="T8" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="U8" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="V8" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="W8" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="X8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="Y8" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="Z8" t="s">
         <v>135</v>
       </c>
       <c r="AA8" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="AB8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AC8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AD8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AE8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="AF8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AG8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM8" t="s">
         <v>138</v>
       </c>
-      <c r="AH8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL8" t="s">
+      <c r="AN8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP8" t="s">
         <v>139</v>
       </c>
-      <c r="AM8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>131</v>
+      <c r="AR8" t="s">
+        <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>109</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
       </c>
       <c r="C9" t="s">
         <v>58</v>
@@ -2566,25 +2593,25 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" t="s">
         <v>112</v>
-      </c>
-      <c r="G9" t="s">
-        <v>120</v>
-      </c>
-      <c r="H9" t="s">
-        <v>113</v>
       </c>
       <c r="I9" t="s">
         <v>55</v>
       </c>
       <c r="J9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" t="s">
+        <v>120</v>
+      </c>
+      <c r="L9" t="s">
         <v>114</v>
-      </c>
-      <c r="K9" t="s">
-        <v>121</v>
-      </c>
-      <c r="L9" t="s">
-        <v>115</v>
       </c>
       <c r="M9" t="s">
         <v>61</v>
@@ -2605,123 +2632,126 @@
         <v>66</v>
       </c>
       <c r="S9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T9" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9" t="s">
+        <v>121</v>
+      </c>
+      <c r="V9" t="s">
+        <v>64</v>
+      </c>
+      <c r="W9" t="s">
+        <v>133</v>
+      </c>
+      <c r="X9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>122</v>
       </c>
-      <c r="U9" t="s">
-        <v>64</v>
-      </c>
-      <c r="V9" t="s">
-        <v>134</v>
-      </c>
-      <c r="W9" t="s">
-        <v>62</v>
-      </c>
-      <c r="X9" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>138</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO9" t="s">
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
         <v>140</v>
       </c>
-      <c r="AQ9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>141</v>
-      </c>
-      <c r="D10" t="s">
-        <v>111</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" t="s">
         <v>124</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" t="s">
         <v>125</v>
       </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>126</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L10" t="s">
+        <v>114</v>
+      </c>
+      <c r="M10" t="s">
         <v>127</v>
       </c>
-      <c r="K10" t="s">
-        <v>142</v>
-      </c>
-      <c r="L10" t="s">
-        <v>115</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
+        <v>62</v>
+      </c>
+      <c r="O10" t="s">
         <v>128</v>
-      </c>
-      <c r="N10" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10" t="s">
-        <v>129</v>
       </c>
       <c r="P10" t="s">
         <v>62</v>
@@ -2733,505 +2763,517 @@
         <v>66</v>
       </c>
       <c r="S10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="T10" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="U10" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="V10" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
       <c r="W10" t="s">
         <v>143</v>
       </c>
       <c r="X10" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="Y10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="Z10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH10" t="s">
         <v>145</v>
       </c>
-      <c r="AA10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE10" t="s">
+      <c r="AI10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR10" t="s">
         <v>149</v>
       </c>
-      <c r="AF10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>147</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ10" t="s">
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>151</v>
       </c>
       <c r="B11" t="s">
         <v>45</v>
       </c>
       <c r="C11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" t="s">
+        <v>152</v>
+      </c>
+      <c r="I11" t="s">
+        <v>153</v>
+      </c>
+      <c r="J11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" t="s">
         <v>156</v>
       </c>
-      <c r="D11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" t="s">
-        <v>152</v>
-      </c>
-      <c r="H11" t="s">
-        <v>153</v>
-      </c>
-      <c r="I11" t="s">
-        <v>154</v>
-      </c>
-      <c r="J11" t="s">
-        <v>155</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>157</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" t="s">
         <v>158</v>
       </c>
-      <c r="M11" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q11" t="s">
         <v>159</v>
-      </c>
-      <c r="O11" t="s">
-        <v>62</v>
-      </c>
-      <c r="P11" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>160</v>
       </c>
       <c r="R11" t="s">
         <v>66</v>
       </c>
       <c r="S11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T11" t="s">
+        <v>64</v>
+      </c>
+      <c r="U11" t="s">
+        <v>160</v>
+      </c>
+      <c r="V11" t="s">
         <v>161</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W11" t="s">
+        <v>62</v>
+      </c>
+      <c r="X11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA11" t="s">
         <v>162</v>
       </c>
-      <c r="V11" t="s">
-        <v>62</v>
-      </c>
-      <c r="W11" t="s">
-        <v>62</v>
-      </c>
-      <c r="X11" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z11" t="s">
+      <c r="AB11" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC11" t="s">
         <v>163</v>
       </c>
-      <c r="AA11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB11" t="s">
+      <c r="AD11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH11" t="s">
         <v>164</v>
       </c>
-      <c r="AC11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG11" t="s">
+      <c r="AI11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>165</v>
       </c>
-      <c r="AH11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP11" t="s">
+      <c r="AR11" t="s">
         <v>166</v>
       </c>
-      <c r="AQ11" t="s">
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>168</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" t="s">
         <v>170</v>
       </c>
-      <c r="G12" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
+        <v>173</v>
+      </c>
+      <c r="K12" t="s">
+        <v>174</v>
+      </c>
+      <c r="L12" t="s">
         <v>176</v>
       </c>
-      <c r="I12" t="s">
-        <v>171</v>
-      </c>
-      <c r="J12" t="s">
-        <v>174</v>
-      </c>
-      <c r="K12" t="s">
-        <v>175</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
+        <v>176</v>
+      </c>
+      <c r="N12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O12" t="s">
+        <v>176</v>
+      </c>
+      <c r="P12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>64</v>
+      </c>
+      <c r="R12" t="s">
         <v>177</v>
       </c>
-      <c r="M12" t="s">
-        <v>177</v>
-      </c>
-      <c r="N12" t="s">
-        <v>62</v>
-      </c>
-      <c r="O12" t="s">
-        <v>177</v>
-      </c>
-      <c r="P12" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>64</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
+        <v>62</v>
+      </c>
+      <c r="T12" t="s">
+        <v>64</v>
+      </c>
+      <c r="U12" t="s">
+        <v>182</v>
+      </c>
+      <c r="V12" t="s">
+        <v>68</v>
+      </c>
+      <c r="W12" t="s">
         <v>178</v>
       </c>
-      <c r="S12" t="s">
-        <v>64</v>
-      </c>
-      <c r="T12" t="s">
+      <c r="X12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>181</v>
+      </c>
+      <c r="AR12" t="s">
         <v>183</v>
       </c>
-      <c r="U12" t="s">
-        <v>68</v>
-      </c>
-      <c r="V12" t="s">
-        <v>179</v>
-      </c>
-      <c r="W12" t="s">
-        <v>62</v>
-      </c>
-      <c r="X12" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>180</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>181</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>182</v>
-      </c>
-      <c r="AQ12" t="s">
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>185</v>
       </c>
-      <c r="B13" t="s">
-        <v>186</v>
-      </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
+        <v>188</v>
+      </c>
+      <c r="G13" t="s">
         <v>189</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" t="s">
         <v>190</v>
       </c>
-      <c r="H13" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>191</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" t="s">
+        <v>114</v>
+      </c>
+      <c r="M13" t="s">
         <v>192</v>
       </c>
-      <c r="K13" t="s">
-        <v>99</v>
-      </c>
-      <c r="L13" t="s">
-        <v>115</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" t="s">
         <v>193</v>
       </c>
-      <c r="N13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>64</v>
+      </c>
+      <c r="R13" t="s">
+        <v>66</v>
+      </c>
+      <c r="S13" t="s">
+        <v>62</v>
+      </c>
+      <c r="T13" t="s">
+        <v>68</v>
+      </c>
+      <c r="U13" t="s">
+        <v>62</v>
+      </c>
+      <c r="V13" t="s">
+        <v>205</v>
+      </c>
+      <c r="W13" t="s">
+        <v>195</v>
+      </c>
+      <c r="X13" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF13" t="s">
         <v>194</v>
       </c>
-      <c r="P13" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R13" t="s">
-        <v>178</v>
-      </c>
-      <c r="S13" t="s">
-        <v>68</v>
-      </c>
-      <c r="T13" t="s">
-        <v>62</v>
-      </c>
-      <c r="U13" t="s">
-        <v>206</v>
-      </c>
-      <c r="V13" t="s">
+      <c r="AG13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH13" t="s">
         <v>196</v>
       </c>
-      <c r="W13" t="s">
-        <v>143</v>
-      </c>
-      <c r="X13" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>195</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG13" t="s">
+      <c r="AI13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO13" t="s">
         <v>197</v>
       </c>
-      <c r="AH13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN13" t="s">
+      <c r="AP13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ13" t="s">
         <v>198</v>
       </c>
-      <c r="AO13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP13" t="s">
+      <c r="AR13" t="s">
         <v>199</v>
       </c>
-      <c r="AQ13" t="s">
-        <v>200</v>
-      </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
       <c r="F14" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14" t="s">
         <v>201</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>202</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>203</v>
-      </c>
-      <c r="J14" t="s">
-        <v>204</v>
       </c>
       <c r="K14" t="s">
         <v>59</v>
       </c>
       <c r="L14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M14" t="s">
+        <v>192</v>
+      </c>
+      <c r="N14" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" t="s">
         <v>193</v>
       </c>
-      <c r="N14" t="s">
-        <v>62</v>
-      </c>
-      <c r="O14" t="s">
-        <v>194</v>
-      </c>
       <c r="P14" t="s">
         <v>62</v>
       </c>
@@ -3239,121 +3281,124 @@
         <v>64</v>
       </c>
       <c r="R14" t="s">
-        <v>178</v>
+        <v>66</v>
       </c>
       <c r="S14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T14" t="s">
+        <v>64</v>
+      </c>
+      <c r="U14" t="s">
+        <v>209</v>
+      </c>
+      <c r="V14" t="s">
+        <v>206</v>
+      </c>
+      <c r="W14" t="s">
+        <v>207</v>
+      </c>
+      <c r="X14" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD14" t="s">
         <v>210</v>
       </c>
-      <c r="U14" t="s">
-        <v>207</v>
-      </c>
-      <c r="V14" t="s">
-        <v>208</v>
-      </c>
-      <c r="W14" t="s">
-        <v>209</v>
-      </c>
-      <c r="X14" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y14" t="s">
+      <c r="AE14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>210</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>211</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR14" t="s">
         <v>214</v>
       </c>
-      <c r="Z14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>211</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>211</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>212</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>215</v>
-      </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" t="s">
         <v>201</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>202</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>203</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>204</v>
       </c>
-      <c r="K15" t="s">
-        <v>205</v>
-      </c>
       <c r="L15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M15" t="s">
+        <v>192</v>
+      </c>
+      <c r="N15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O15" t="s">
         <v>193</v>
       </c>
-      <c r="N15" t="s">
-        <v>62</v>
-      </c>
-      <c r="O15" t="s">
-        <v>194</v>
-      </c>
       <c r="P15" t="s">
         <v>62</v>
       </c>
@@ -3361,76 +3406,79 @@
         <v>64</v>
       </c>
       <c r="R15" t="s">
-        <v>178</v>
+        <v>66</v>
       </c>
       <c r="S15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T15" t="s">
+        <v>64</v>
+      </c>
+      <c r="U15" t="s">
+        <v>209</v>
+      </c>
+      <c r="V15" t="s">
+        <v>206</v>
+      </c>
+      <c r="W15" t="s">
+        <v>207</v>
+      </c>
+      <c r="X15" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD15" t="s">
         <v>210</v>
       </c>
-      <c r="U15" t="s">
-        <v>207</v>
-      </c>
-      <c r="V15" t="s">
-        <v>208</v>
-      </c>
-      <c r="W15" t="s">
-        <v>209</v>
-      </c>
-      <c r="X15" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y15" t="s">
+      <c r="AE15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>210</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>211</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR15" t="s">
         <v>214</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>211</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>211</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>212</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing entry for delpierre
</commit_message>
<xml_diff>
--- a/data/submittedround6/grephon table Alana and Cat final round.xlsx
+++ b/data/submittedround6/grephon table Alana and Cat final round.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.chamberlain/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.chamberlain/Documents/git/grephon/data/submittedround6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2738EE2-5AFF-8143-8865-AA29582E8D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531D2015-3C39-4E42-92E6-02A96673BB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="760" windowWidth="30880" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="217">
   <si>
     <t>paper_id</t>
   </si>
@@ -1533,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13:R15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3253,8 +3253,11 @@
       <c r="G14" t="s">
         <v>201</v>
       </c>
+      <c r="H14" t="s">
+        <v>202</v>
+      </c>
       <c r="I14" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="J14" t="s">
         <v>203</v>
@@ -3378,8 +3381,11 @@
       <c r="G15" t="s">
         <v>201</v>
       </c>
+      <c r="H15" t="s">
+        <v>202</v>
+      </c>
       <c r="I15" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="J15" t="s">
         <v>203</v>

</xml_diff>